<commit_message>
corrrected medium columnn to conform to stnadard
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_0659.xlsx
+++ b/bioSample/bioSample_0659.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/bioSample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA8EAEA-7751-334F-BB67-0BC0DD8B41D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC7A511-6169-6645-8DA1-6493AE424480}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16820" yWindow="460" windowWidth="33600" windowHeight="18940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="34">
   <si>
     <t>harvestDate</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>DMEM</t>
+  </si>
+  <si>
+    <t>medium</t>
   </si>
 </sst>
 </file>
@@ -485,7 +488,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -512,7 +515,9 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1"/>
+      <c r="H1" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>

</xml_diff>